<commit_message>
update 1 at 31 may
</commit_message>
<xml_diff>
--- a/Consolidate Excel Sheet.xlsx
+++ b/Consolidate Excel Sheet.xlsx
@@ -1571,7 +1571,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,6 +1843,9 @@
       <c r="E12" s="6">
         <v>2019</v>
       </c>
+      <c r="H12" s="10">
+        <v>124</v>
+      </c>
       <c r="I12" s="6" t="s">
         <v>55</v>
       </c>

</xml_diff>